<commit_message>
dc_pod_v010 missing factors fixed
</commit_message>
<xml_diff>
--- a/storages/project_convector/dc_pod_v010/dc.xlsx
+++ b/storages/project_convector/dc_pod_v010/dc.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0798f53157368e05/RAMP/IP-02/new_OSTRTA/macro/macro/data/dc_pod/dc_pod_v010/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{AFF43772-47AF-4283-A599-C691D98783E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89947FBC-81D8-464E-B7F0-A8EC8047EC62}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{AFF43772-47AF-4283-A599-C691D98783E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A396E03-566F-4FE9-8EB5-2E8CB04B0E93}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tier_I" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="457">
   <si>
     <t>A091RC1Q027SBEA</t>
   </si>
@@ -1331,6 +1345,66 @@
   </si>
   <si>
     <t>csv</t>
+  </si>
+  <si>
+    <t>IUES.L</t>
+  </si>
+  <si>
+    <t>IUIT.L</t>
+  </si>
+  <si>
+    <t>global groups:</t>
+  </si>
+  <si>
+    <t>&gt; macro: economic activity</t>
+  </si>
+  <si>
+    <t>&gt; macro: demand</t>
+  </si>
+  <si>
+    <t>&gt; macro: revenues</t>
+  </si>
+  <si>
+    <t>&gt; macro: liquidity impulse</t>
+  </si>
+  <si>
+    <t>&gt; capital: yields in different classes</t>
+  </si>
+  <si>
+    <t>&gt; commodities: prices</t>
+  </si>
+  <si>
+    <t>https://finance.yahoo.com/quote/IUES.L/history/</t>
+  </si>
+  <si>
+    <t>iShares S&amp;P 500 Energy Sector UCITS ETF USD (Acc)</t>
+  </si>
+  <si>
+    <t>https://finance.yahoo.com/quote/IUIT.L/history/</t>
+  </si>
+  <si>
+    <t>iShares S&amp;P 500 Information Technology Sector UCITS ETF USD (Acc)</t>
+  </si>
+  <si>
+    <t>https://www.etf.com/etfanalytics/etf-fund-flows-tool-result?tickers=IVV%2C&amp;startDate=2007-07-02&amp;endDate=2024-08-06&amp;frequency=MONTHLY</t>
+  </si>
+  <si>
+    <t>Calculated manually as flows(VOO + IVV + SPY + VTI + QQQ)</t>
+  </si>
+  <si>
+    <t>SNPF</t>
+  </si>
+  <si>
+    <t>W-MON</t>
+  </si>
+  <si>
+    <t>DTWEXBGS</t>
+  </si>
+  <si>
+    <t>Nominal Broad U.S. Dollar Index</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/DTWEXBGS</t>
   </si>
 </sst>
 </file>
@@ -1586,6 +1660,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1905,10 +1983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:I145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="J145" sqref="J145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1917,7 +1995,9 @@
     <col min="2" max="3" width="11.88671875" customWidth="1"/>
     <col min="4" max="4" width="46.21875" customWidth="1"/>
     <col min="5" max="5" width="18.5546875" customWidth="1"/>
-    <col min="6" max="18" width="11.88671875" customWidth="1"/>
+    <col min="6" max="9" width="11.88671875" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="18" width="11.88671875" customWidth="1"/>
     <col min="19" max="19" width="51.77734375" customWidth="1"/>
     <col min="20" max="20" width="8.88671875" customWidth="1"/>
   </cols>
@@ -5327,6 +5407,9 @@
       <c r="F131" t="s">
         <v>433</v>
       </c>
+      <c r="G131" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="H131">
         <v>0</v>
       </c>
@@ -5350,6 +5433,9 @@
       <c r="F132" t="s">
         <v>433</v>
       </c>
+      <c r="G132" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="H132">
         <v>0</v>
       </c>
@@ -5373,6 +5459,9 @@
       <c r="F133" t="s">
         <v>433</v>
       </c>
+      <c r="G133" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="H133">
         <v>0</v>
       </c>
@@ -5396,6 +5485,9 @@
       <c r="F134" t="s">
         <v>433</v>
       </c>
+      <c r="G134" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="H134">
         <v>0</v>
       </c>
@@ -5419,6 +5511,9 @@
       <c r="F135" t="s">
         <v>433</v>
       </c>
+      <c r="G135" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="H135">
         <v>0</v>
       </c>
@@ -5442,6 +5537,9 @@
       <c r="F136" t="s">
         <v>433</v>
       </c>
+      <c r="G136" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="H136">
         <v>0</v>
       </c>
@@ -5465,6 +5563,9 @@
       <c r="F137" t="s">
         <v>433</v>
       </c>
+      <c r="G137" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="H137">
         <v>0</v>
       </c>
@@ -5488,6 +5589,9 @@
       <c r="F138" t="s">
         <v>433</v>
       </c>
+      <c r="G138" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="H138">
         <v>0</v>
       </c>
@@ -5511,6 +5615,9 @@
       <c r="F139" t="s">
         <v>433</v>
       </c>
+      <c r="G139" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="H139">
         <v>0</v>
       </c>
@@ -5534,6 +5641,9 @@
       <c r="F140" t="s">
         <v>433</v>
       </c>
+      <c r="G140" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="H140">
         <v>0</v>
       </c>
@@ -5557,7 +5667,114 @@
       <c r="F141" t="s">
         <v>433</v>
       </c>
+      <c r="G141" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="H141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>437</v>
+      </c>
+      <c r="B142" t="s">
+        <v>447</v>
+      </c>
+      <c r="C142" t="s">
+        <v>429</v>
+      </c>
+      <c r="D142" t="s">
+        <v>446</v>
+      </c>
+      <c r="E142" t="s">
+        <v>436</v>
+      </c>
+      <c r="F142" t="s">
+        <v>431</v>
+      </c>
+      <c r="G142" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="H142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>438</v>
+      </c>
+      <c r="B143" t="s">
+        <v>449</v>
+      </c>
+      <c r="C143" t="s">
+        <v>429</v>
+      </c>
+      <c r="D143" t="s">
+        <v>448</v>
+      </c>
+      <c r="E143" t="s">
+        <v>436</v>
+      </c>
+      <c r="F143" t="s">
+        <v>431</v>
+      </c>
+      <c r="G143" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="H143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>452</v>
+      </c>
+      <c r="B144" t="s">
+        <v>451</v>
+      </c>
+      <c r="C144" t="s">
+        <v>429</v>
+      </c>
+      <c r="D144" t="s">
+        <v>450</v>
+      </c>
+      <c r="E144" t="s">
+        <v>436</v>
+      </c>
+      <c r="F144" t="s">
+        <v>453</v>
+      </c>
+      <c r="G144" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="H144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>454</v>
+      </c>
+      <c r="B145" t="s">
+        <v>455</v>
+      </c>
+      <c r="C145" t="s">
+        <v>429</v>
+      </c>
+      <c r="D145" t="s">
+        <v>456</v>
+      </c>
+      <c r="E145" t="s">
+        <v>436</v>
+      </c>
+      <c r="F145" t="s">
+        <v>433</v>
+      </c>
+      <c r="G145" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="H145">
         <v>0</v>
       </c>
     </row>
@@ -5696,4 +5913,54 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DF86C7-82B7-4F6E-939E-BF588D52CF27}">
+  <dimension ref="B4:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>444</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
dc_pod improvements: corrected non-compliant separator in DTWEXBGS; assigned appropriate frequencies to TERMCBCCALLNS and TERMCBCCINTNS; corrected project status
</commit_message>
<xml_diff>
--- a/storages/project_convector/dc_pod_v010/dc.xlsx
+++ b/storages/project_convector/dc_pod_v010/dc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0798f53157368e05/RAMP/IP-02/new_OSTRTA/macro/macro/data/dc_pod/dc_pod_v010/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0798f53157368e05/RAMP/IP-02/new_OSTRTA/convey/convey/storages/project_convector/dc_pod_v010/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{AFF43772-47AF-4283-A599-C691D98783E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A396E03-566F-4FE9-8EB5-2E8CB04B0E93}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{AFF43772-47AF-4283-A599-C691D98783E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB5DFF64-2EEC-475D-AA0E-5EC348D24B12}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="457">
   <si>
     <t>A091RC1Q027SBEA</t>
   </si>
@@ -1338,9 +1338,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>actual frequency is quarterly; frequency specification is adjusted due to technical reasons</t>
-  </si>
-  <si>
     <t>reader</t>
   </si>
   <si>
@@ -1405,6 +1402,9 @@
   </si>
   <si>
     <t>https://fred.stlouisfed.org/series/DTWEXBGS</t>
+  </si>
+  <si>
+    <t>QS-NOV</t>
   </si>
 </sst>
 </file>
@@ -1660,10 +1660,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1985,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J145" sqref="J145"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I122" sqref="I122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2016,7 +2012,7 @@
         <v>421</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>426</v>
@@ -2045,7 +2041,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F2" t="s">
         <v>430</v>
@@ -2072,7 +2068,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F3" t="s">
         <v>431</v>
@@ -2098,7 +2094,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F4" t="s">
         <v>430</v>
@@ -2124,7 +2120,7 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F5" t="s">
         <v>431</v>
@@ -2150,7 +2146,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F6" t="s">
         <v>431</v>
@@ -2176,7 +2172,7 @@
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F7" t="s">
         <v>431</v>
@@ -2202,7 +2198,7 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F8" t="s">
         <v>431</v>
@@ -2228,7 +2224,7 @@
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F9" t="s">
         <v>431</v>
@@ -2254,7 +2250,7 @@
         <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F10" t="s">
         <v>433</v>
@@ -2280,7 +2276,7 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F11" t="s">
         <v>433</v>
@@ -2306,7 +2302,7 @@
         <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F12" t="s">
         <v>433</v>
@@ -2332,7 +2328,7 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F13" t="s">
         <v>433</v>
@@ -2358,7 +2354,7 @@
         <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F14" t="s">
         <v>433</v>
@@ -2384,7 +2380,7 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F15" t="s">
         <v>433</v>
@@ -2410,7 +2406,7 @@
         <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F16" t="s">
         <v>431</v>
@@ -2436,7 +2432,7 @@
         <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F17" t="s">
         <v>431</v>
@@ -2462,7 +2458,7 @@
         <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F18" t="s">
         <v>431</v>
@@ -2488,7 +2484,7 @@
         <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F19" t="s">
         <v>431</v>
@@ -2514,7 +2510,7 @@
         <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F20" t="s">
         <v>431</v>
@@ -2540,7 +2536,7 @@
         <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F21" t="s">
         <v>431</v>
@@ -2566,7 +2562,7 @@
         <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F22" t="s">
         <v>431</v>
@@ -2592,7 +2588,7 @@
         <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F23" t="s">
         <v>431</v>
@@ -2618,7 +2614,7 @@
         <v>68</v>
       </c>
       <c r="E24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F24" t="s">
         <v>431</v>
@@ -2644,7 +2640,7 @@
         <v>71</v>
       </c>
       <c r="E25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F25" t="s">
         <v>431</v>
@@ -2670,7 +2666,7 @@
         <v>74</v>
       </c>
       <c r="E26" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F26" t="s">
         <v>432</v>
@@ -2696,7 +2692,7 @@
         <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F27" t="s">
         <v>431</v>
@@ -2722,7 +2718,7 @@
         <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F28" t="s">
         <v>431</v>
@@ -2748,7 +2744,7 @@
         <v>83</v>
       </c>
       <c r="E29" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F29" t="s">
         <v>430</v>
@@ -2774,7 +2770,7 @@
         <v>86</v>
       </c>
       <c r="E30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F30" t="s">
         <v>430</v>
@@ -2800,7 +2796,7 @@
         <v>89</v>
       </c>
       <c r="E31" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F31" t="s">
         <v>432</v>
@@ -2826,7 +2822,7 @@
         <v>92</v>
       </c>
       <c r="E32" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F32" t="s">
         <v>430</v>
@@ -2852,7 +2848,7 @@
         <v>95</v>
       </c>
       <c r="E33" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F33" t="s">
         <v>431</v>
@@ -2878,7 +2874,7 @@
         <v>98</v>
       </c>
       <c r="E34" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F34" t="s">
         <v>432</v>
@@ -2904,7 +2900,7 @@
         <v>101</v>
       </c>
       <c r="E35" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F35" t="s">
         <v>433</v>
@@ -2930,7 +2926,7 @@
         <v>104</v>
       </c>
       <c r="E36" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F36" t="s">
         <v>433</v>
@@ -2956,7 +2952,7 @@
         <v>107</v>
       </c>
       <c r="E37" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F37" t="s">
         <v>431</v>
@@ -2982,7 +2978,7 @@
         <v>110</v>
       </c>
       <c r="E38" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F38" t="s">
         <v>431</v>
@@ -3008,7 +3004,7 @@
         <v>113</v>
       </c>
       <c r="E39" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F39" t="s">
         <v>431</v>
@@ -3034,7 +3030,7 @@
         <v>116</v>
       </c>
       <c r="E40" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F40" t="s">
         <v>431</v>
@@ -3060,7 +3056,7 @@
         <v>119</v>
       </c>
       <c r="E41" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F41" t="s">
         <v>431</v>
@@ -3086,7 +3082,7 @@
         <v>122</v>
       </c>
       <c r="E42" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F42" t="s">
         <v>430</v>
@@ -3112,7 +3108,7 @@
         <v>125</v>
       </c>
       <c r="E43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F43" t="s">
         <v>431</v>
@@ -3138,7 +3134,7 @@
         <v>128</v>
       </c>
       <c r="E44" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F44" t="s">
         <v>431</v>
@@ -3164,7 +3160,7 @@
         <v>131</v>
       </c>
       <c r="E45" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F45" t="s">
         <v>432</v>
@@ -3190,7 +3186,7 @@
         <v>134</v>
       </c>
       <c r="E46" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F46" t="s">
         <v>431</v>
@@ -3216,7 +3212,7 @@
         <v>137</v>
       </c>
       <c r="E47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F47" t="s">
         <v>431</v>
@@ -3242,7 +3238,7 @@
         <v>140</v>
       </c>
       <c r="E48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F48" t="s">
         <v>430</v>
@@ -3268,7 +3264,7 @@
         <v>143</v>
       </c>
       <c r="E49" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F49" t="s">
         <v>430</v>
@@ -3294,7 +3290,7 @@
         <v>146</v>
       </c>
       <c r="E50" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F50" t="s">
         <v>431</v>
@@ -3320,7 +3316,7 @@
         <v>149</v>
       </c>
       <c r="E51" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F51" t="s">
         <v>430</v>
@@ -3346,7 +3342,7 @@
         <v>152</v>
       </c>
       <c r="E52" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F52" t="s">
         <v>430</v>
@@ -3372,7 +3368,7 @@
         <v>155</v>
       </c>
       <c r="E53" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F53" t="s">
         <v>430</v>
@@ -3398,7 +3394,7 @@
         <v>158</v>
       </c>
       <c r="E54" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F54" t="s">
         <v>431</v>
@@ -3424,7 +3420,7 @@
         <v>161</v>
       </c>
       <c r="E55" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F55" t="s">
         <v>431</v>
@@ -3450,7 +3446,7 @@
         <v>164</v>
       </c>
       <c r="E56" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F56" t="s">
         <v>431</v>
@@ -3476,7 +3472,7 @@
         <v>167</v>
       </c>
       <c r="E57" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F57" t="s">
         <v>431</v>
@@ -3502,7 +3498,7 @@
         <v>170</v>
       </c>
       <c r="E58" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F58" t="s">
         <v>431</v>
@@ -3528,7 +3524,7 @@
         <v>173</v>
       </c>
       <c r="E59" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F59" t="s">
         <v>431</v>
@@ -3554,7 +3550,7 @@
         <v>176</v>
       </c>
       <c r="E60" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F60" t="s">
         <v>431</v>
@@ -3580,7 +3576,7 @@
         <v>179</v>
       </c>
       <c r="E61" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F61" t="s">
         <v>430</v>
@@ -3606,7 +3602,7 @@
         <v>182</v>
       </c>
       <c r="E62" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F62" t="s">
         <v>431</v>
@@ -3632,7 +3628,7 @@
         <v>185</v>
       </c>
       <c r="E63" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F63" t="s">
         <v>430</v>
@@ -3658,7 +3654,7 @@
         <v>188</v>
       </c>
       <c r="E64" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F64" t="s">
         <v>430</v>
@@ -3684,7 +3680,7 @@
         <v>191</v>
       </c>
       <c r="E65" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F65" t="s">
         <v>430</v>
@@ -3710,7 +3706,7 @@
         <v>194</v>
       </c>
       <c r="E66" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F66" t="s">
         <v>430</v>
@@ -3736,7 +3732,7 @@
         <v>197</v>
       </c>
       <c r="E67" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F67" t="s">
         <v>431</v>
@@ -3762,7 +3758,7 @@
         <v>200</v>
       </c>
       <c r="E68" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F68" t="s">
         <v>431</v>
@@ -3788,7 +3784,7 @@
         <v>203</v>
       </c>
       <c r="E69" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F69" t="s">
         <v>431</v>
@@ -3814,7 +3810,7 @@
         <v>206</v>
       </c>
       <c r="E70" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F70" t="s">
         <v>431</v>
@@ -3840,7 +3836,7 @@
         <v>209</v>
       </c>
       <c r="E71" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F71" t="s">
         <v>433</v>
@@ -3864,7 +3860,7 @@
         <v>212</v>
       </c>
       <c r="E72" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F72" t="s">
         <v>431</v>
@@ -3890,7 +3886,7 @@
         <v>215</v>
       </c>
       <c r="E73" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F73" t="s">
         <v>431</v>
@@ -3916,7 +3912,7 @@
         <v>218</v>
       </c>
       <c r="E74" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F74" t="s">
         <v>431</v>
@@ -3942,7 +3938,7 @@
         <v>221</v>
       </c>
       <c r="E75" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F75" t="s">
         <v>431</v>
@@ -3968,7 +3964,7 @@
         <v>224</v>
       </c>
       <c r="E76" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F76" t="s">
         <v>431</v>
@@ -3994,7 +3990,7 @@
         <v>227</v>
       </c>
       <c r="E77" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F77" t="s">
         <v>431</v>
@@ -4020,7 +4016,7 @@
         <v>230</v>
       </c>
       <c r="E78" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F78" t="s">
         <v>430</v>
@@ -4046,7 +4042,7 @@
         <v>233</v>
       </c>
       <c r="E79" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F79" t="s">
         <v>431</v>
@@ -4072,7 +4068,7 @@
         <v>236</v>
       </c>
       <c r="E80" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F80" t="s">
         <v>431</v>
@@ -4098,7 +4094,7 @@
         <v>239</v>
       </c>
       <c r="E81" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F81" t="s">
         <v>431</v>
@@ -4124,7 +4120,7 @@
         <v>242</v>
       </c>
       <c r="E82" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F82" t="s">
         <v>431</v>
@@ -4150,7 +4146,7 @@
         <v>245</v>
       </c>
       <c r="E83" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F83" t="s">
         <v>431</v>
@@ -4176,7 +4172,7 @@
         <v>248</v>
       </c>
       <c r="E84" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F84" t="s">
         <v>431</v>
@@ -4202,7 +4198,7 @@
         <v>251</v>
       </c>
       <c r="E85" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F85" t="s">
         <v>431</v>
@@ -4228,7 +4224,7 @@
         <v>254</v>
       </c>
       <c r="E86" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F86" t="s">
         <v>431</v>
@@ -4254,7 +4250,7 @@
         <v>257</v>
       </c>
       <c r="E87" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F87" t="s">
         <v>431</v>
@@ -4280,7 +4276,7 @@
         <v>260</v>
       </c>
       <c r="E88" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F88" t="s">
         <v>431</v>
@@ -4306,7 +4302,7 @@
         <v>263</v>
       </c>
       <c r="E89" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F89" t="s">
         <v>431</v>
@@ -4332,7 +4328,7 @@
         <v>266</v>
       </c>
       <c r="E90" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F90" t="s">
         <v>431</v>
@@ -4358,7 +4354,7 @@
         <v>269</v>
       </c>
       <c r="E91" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F91" t="s">
         <v>431</v>
@@ -4384,7 +4380,7 @@
         <v>272</v>
       </c>
       <c r="E92" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F92" t="s">
         <v>431</v>
@@ -4410,7 +4406,7 @@
         <v>275</v>
       </c>
       <c r="E93" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F93" t="s">
         <v>431</v>
@@ -4436,7 +4432,7 @@
         <v>278</v>
       </c>
       <c r="E94" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F94" t="s">
         <v>430</v>
@@ -4462,7 +4458,7 @@
         <v>281</v>
       </c>
       <c r="E95" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F95" t="s">
         <v>430</v>
@@ -4488,7 +4484,7 @@
         <v>284</v>
       </c>
       <c r="E96" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F96" t="s">
         <v>431</v>
@@ -4514,7 +4510,7 @@
         <v>287</v>
       </c>
       <c r="E97" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F97" t="s">
         <v>430</v>
@@ -4540,7 +4536,7 @@
         <v>290</v>
       </c>
       <c r="E98" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F98" t="s">
         <v>430</v>
@@ -4566,7 +4562,7 @@
         <v>293</v>
       </c>
       <c r="E99" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F99" t="s">
         <v>431</v>
@@ -4592,7 +4588,7 @@
         <v>296</v>
       </c>
       <c r="E100" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F100" t="s">
         <v>431</v>
@@ -4618,7 +4614,7 @@
         <v>299</v>
       </c>
       <c r="E101" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F101" t="s">
         <v>431</v>
@@ -4644,7 +4640,7 @@
         <v>302</v>
       </c>
       <c r="E102" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F102" t="s">
         <v>431</v>
@@ -4670,7 +4666,7 @@
         <v>305</v>
       </c>
       <c r="E103" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F103" t="s">
         <v>431</v>
@@ -4696,7 +4692,7 @@
         <v>308</v>
       </c>
       <c r="E104" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F104" t="s">
         <v>431</v>
@@ -4722,7 +4718,7 @@
         <v>311</v>
       </c>
       <c r="E105" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F105" t="s">
         <v>431</v>
@@ -4748,7 +4744,7 @@
         <v>314</v>
       </c>
       <c r="E106" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F106" t="s">
         <v>431</v>
@@ -4774,7 +4770,7 @@
         <v>317</v>
       </c>
       <c r="E107" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F107" t="s">
         <v>431</v>
@@ -4800,7 +4796,7 @@
         <v>320</v>
       </c>
       <c r="E108" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F108" t="s">
         <v>431</v>
@@ -4826,7 +4822,7 @@
         <v>323</v>
       </c>
       <c r="E109" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F109" t="s">
         <v>431</v>
@@ -4852,7 +4848,7 @@
         <v>326</v>
       </c>
       <c r="E110" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F110" t="s">
         <v>431</v>
@@ -4878,7 +4874,7 @@
         <v>329</v>
       </c>
       <c r="E111" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F111" t="s">
         <v>431</v>
@@ -4904,7 +4900,7 @@
         <v>332</v>
       </c>
       <c r="E112" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F112" t="s">
         <v>431</v>
@@ -4916,7 +4912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>333</v>
       </c>
@@ -4930,7 +4926,7 @@
         <v>335</v>
       </c>
       <c r="E113" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F113" t="s">
         <v>431</v>
@@ -4942,7 +4938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>336</v>
       </c>
@@ -4956,7 +4952,7 @@
         <v>338</v>
       </c>
       <c r="E114" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F114" t="s">
         <v>431</v>
@@ -4968,7 +4964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>339</v>
       </c>
@@ -4982,7 +4978,7 @@
         <v>341</v>
       </c>
       <c r="E115" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F115" t="s">
         <v>431</v>
@@ -4994,7 +4990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>342</v>
       </c>
@@ -5008,7 +5004,7 @@
         <v>344</v>
       </c>
       <c r="E116" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F116" t="s">
         <v>431</v>
@@ -5020,7 +5016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>345</v>
       </c>
@@ -5034,7 +5030,7 @@
         <v>347</v>
       </c>
       <c r="E117" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F117" t="s">
         <v>431</v>
@@ -5046,7 +5042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>348</v>
       </c>
@@ -5060,7 +5056,7 @@
         <v>350</v>
       </c>
       <c r="E118" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F118" t="s">
         <v>431</v>
@@ -5072,7 +5068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>351</v>
       </c>
@@ -5086,7 +5082,7 @@
         <v>353</v>
       </c>
       <c r="E119" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F119" t="s">
         <v>431</v>
@@ -5098,7 +5094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>354</v>
       </c>
@@ -5112,7 +5108,7 @@
         <v>356</v>
       </c>
       <c r="E120" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F120" t="s">
         <v>431</v>
@@ -5124,7 +5120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>357</v>
       </c>
@@ -5138,10 +5134,10 @@
         <v>359</v>
       </c>
       <c r="E121" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F121" t="s">
-        <v>431</v>
+        <v>456</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>428</v>
@@ -5149,11 +5145,8 @@
       <c r="H121">
         <v>2</v>
       </c>
-      <c r="I121" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>360</v>
       </c>
@@ -5167,10 +5160,10 @@
         <v>362</v>
       </c>
       <c r="E122" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F122" t="s">
-        <v>431</v>
+        <v>456</v>
       </c>
       <c r="G122" s="4" t="s">
         <v>428</v>
@@ -5178,11 +5171,8 @@
       <c r="H122">
         <v>2</v>
       </c>
-      <c r="I122" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>363</v>
       </c>
@@ -5196,7 +5186,7 @@
         <v>364</v>
       </c>
       <c r="E123" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F123" t="s">
         <v>433</v>
@@ -5206,7 +5196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>365</v>
       </c>
@@ -5220,7 +5210,7 @@
         <v>367</v>
       </c>
       <c r="E124" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F124" t="s">
         <v>431</v>
@@ -5232,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>368</v>
       </c>
@@ -5246,7 +5236,7 @@
         <v>370</v>
       </c>
       <c r="E125" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F125" t="s">
         <v>431</v>
@@ -5258,7 +5248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>371</v>
       </c>
@@ -5272,7 +5262,7 @@
         <v>373</v>
       </c>
       <c r="E126" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F126" t="s">
         <v>431</v>
@@ -5284,7 +5274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>374</v>
       </c>
@@ -5298,7 +5288,7 @@
         <v>376</v>
       </c>
       <c r="E127" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F127" t="s">
         <v>431</v>
@@ -5310,7 +5300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>377</v>
       </c>
@@ -5324,7 +5314,7 @@
         <v>379</v>
       </c>
       <c r="E128" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F128" t="s">
         <v>431</v>
@@ -5350,7 +5340,7 @@
         <v>382</v>
       </c>
       <c r="E129" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F129" t="s">
         <v>431</v>
@@ -5376,7 +5366,7 @@
         <v>385</v>
       </c>
       <c r="E130" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F130" t="s">
         <v>430</v>
@@ -5402,7 +5392,7 @@
         <v>388</v>
       </c>
       <c r="E131" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F131" t="s">
         <v>433</v>
@@ -5428,7 +5418,7 @@
         <v>391</v>
       </c>
       <c r="E132" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F132" t="s">
         <v>433</v>
@@ -5454,7 +5444,7 @@
         <v>394</v>
       </c>
       <c r="E133" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F133" t="s">
         <v>433</v>
@@ -5480,7 +5470,7 @@
         <v>397</v>
       </c>
       <c r="E134" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F134" t="s">
         <v>433</v>
@@ -5506,7 +5496,7 @@
         <v>400</v>
       </c>
       <c r="E135" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F135" t="s">
         <v>433</v>
@@ -5532,7 +5522,7 @@
         <v>403</v>
       </c>
       <c r="E136" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F136" t="s">
         <v>433</v>
@@ -5558,7 +5548,7 @@
         <v>406</v>
       </c>
       <c r="E137" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F137" t="s">
         <v>433</v>
@@ -5584,7 +5574,7 @@
         <v>409</v>
       </c>
       <c r="E138" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F138" t="s">
         <v>433</v>
@@ -5610,7 +5600,7 @@
         <v>412</v>
       </c>
       <c r="E139" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F139" t="s">
         <v>433</v>
@@ -5636,7 +5626,7 @@
         <v>415</v>
       </c>
       <c r="E140" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F140" t="s">
         <v>433</v>
@@ -5662,7 +5652,7 @@
         <v>418</v>
       </c>
       <c r="E141" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F141" t="s">
         <v>433</v>
@@ -5676,19 +5666,19 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B142" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C142" t="s">
         <v>429</v>
       </c>
       <c r="D142" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E142" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F142" t="s">
         <v>431</v>
@@ -5702,19 +5692,19 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B143" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C143" t="s">
         <v>429</v>
       </c>
       <c r="D143" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E143" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F143" t="s">
         <v>431</v>
@@ -5728,22 +5718,22 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>451</v>
+      </c>
+      <c r="B144" t="s">
+        <v>450</v>
+      </c>
+      <c r="C144" t="s">
+        <v>429</v>
+      </c>
+      <c r="D144" t="s">
+        <v>449</v>
+      </c>
+      <c r="E144" t="s">
+        <v>435</v>
+      </c>
+      <c r="F144" t="s">
         <v>452</v>
-      </c>
-      <c r="B144" t="s">
-        <v>451</v>
-      </c>
-      <c r="C144" t="s">
-        <v>429</v>
-      </c>
-      <c r="D144" t="s">
-        <v>450</v>
-      </c>
-      <c r="E144" t="s">
-        <v>436</v>
-      </c>
-      <c r="F144" t="s">
-        <v>453</v>
       </c>
       <c r="G144" s="4" t="s">
         <v>428</v>
@@ -5754,19 +5744,19 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>453</v>
+      </c>
+      <c r="B145" t="s">
         <v>454</v>
       </c>
-      <c r="B145" t="s">
+      <c r="C145" t="s">
+        <v>429</v>
+      </c>
+      <c r="D145" t="s">
         <v>455</v>
       </c>
-      <c r="C145" t="s">
-        <v>429</v>
-      </c>
-      <c r="D145" t="s">
-        <v>456</v>
-      </c>
       <c r="E145" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F145" t="s">
         <v>433</v>
@@ -5927,37 +5917,37 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Specified dc_pod_v010 publication lags
</commit_message>
<xml_diff>
--- a/storages/project_convector/dc_pod_v010/dc.xlsx
+++ b/storages/project_convector/dc_pod_v010/dc.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0798f53157368e05/RAMP/IP-02/new_OSTRTA/convey/convey/storages/project_convector/dc_pod_v010/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{AFF43772-47AF-4283-A599-C691D98783E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB5DFF64-2EEC-475D-AA0E-5EC348D24B12}"/>
+  <xr:revisionPtr revIDLastSave="432" documentId="13_ncr:1_{22F8F620-03E2-48CE-8A04-EB9BE08523DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08E12BB0-9B12-45F3-8B9D-381DB1393DD2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tier_I" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="todo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="558">
   <si>
     <t>A091RC1Q027SBEA</t>
   </si>
@@ -1405,6 +1405,309 @@
   </si>
   <si>
     <t>QS-NOV</t>
+  </si>
+  <si>
+    <t>Next Release Date: Feb 27, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Jan 30, 2025 7:55 AM CST</t>
+  </si>
+  <si>
+    <t>Q4 2024</t>
+  </si>
+  <si>
+    <t>Dec 2024</t>
+  </si>
+  <si>
+    <t>Jan 2025</t>
+  </si>
+  <si>
+    <t>Next Release Date: Feb 24, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Feb 12, 2025 9:01 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 12, 2025</t>
+  </si>
+  <si>
+    <t>Nov 2024</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 7, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Mar 6, 2025 7:51 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Apr 3, 2025</t>
+  </si>
+  <si>
+    <t>Feb 2025</t>
+  </si>
+  <si>
+    <t>Updated: Mar 7, 2025 7:48 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Apr 4, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Mar 7, 2025 7:49 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Mar 3, 2025 3:16 PM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 10, 2025</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 4, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Feb 12, 2025 7:43 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 25, 2025 8:11 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 25, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Feb 12, 2025 7:44 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 12, 2025 7:41 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 27, 2025 7:55 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 27, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Feb 28, 2025 7:45 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 28, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Feb 27, 2025 7:57 AM CST</t>
+  </si>
+  <si>
+    <t>2025-03-06</t>
+  </si>
+  <si>
+    <t>Updated: Mar 7, 2025 3:17 PM CST</t>
+  </si>
+  <si>
+    <t>Updated: Mar 3, 2025 12:38 PM CST</t>
+  </si>
+  <si>
+    <t>Updated: Mar 5, 2025 8:02 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Mar 5, 2025 8:01 AM CST</t>
+  </si>
+  <si>
+    <t>publication lags:</t>
+  </si>
+  <si>
+    <t>&gt; yearly are still in question</t>
+  </si>
+  <si>
+    <t>&gt; quarterly are still in question</t>
+  </si>
+  <si>
+    <t>Updated: Mar 3, 2025 8:02 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Mar 4, 2025 9:26 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Not Available</t>
+  </si>
+  <si>
+    <t>Updated: Mar 3, 2025 3:17 PM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 12, 2025 12:01 PM CST</t>
+  </si>
+  <si>
+    <t>Updated: Sep 19, 2024 2:08 PM CDT</t>
+  </si>
+  <si>
+    <t>Updated: Feb 13, 2025 4:31 PM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 27, 2025 7:58 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 17, 2025 8:01 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Feb 21, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Mar 4, 2025 9:36 AM CST</t>
+  </si>
+  <si>
+    <t>&gt; GS[X] group has strange update dates; some survellience is in order</t>
+  </si>
+  <si>
+    <t>Updated: Aug 1, 2024 7:02 AM CDT</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 3, 2025</t>
+  </si>
+  <si>
+    <t>Q1 2024</t>
+  </si>
+  <si>
+    <t>Updated: Feb 14, 2025 7:37 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 18, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Dec 27, 2024 7:31 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 26, 2025</t>
+  </si>
+  <si>
+    <t>Q3 2024</t>
+  </si>
+  <si>
+    <t>Updated: Mar 3, 2025 10:42 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Jan 13, 2025 9:55 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 24, 2025 8:39 AM CST</t>
+  </si>
+  <si>
+    <t>&gt; I'd replace interest rates group with something more decent &amp; oriented on relevant markets (EU, Japan, etc)</t>
+  </si>
+  <si>
+    <t>Updated: Feb 17, 2025 2:16 PM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 4, 2025 9:06 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 11, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Feb 12, 2025 2:16 PM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 21, 2025 10:01 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 14, 2025 9:07 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 17, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Jan 27, 2025 9:01 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Feb 26, 2025</t>
+  </si>
+  <si>
+    <t>&gt; think of replacing rigid low-frequency series with alternatively sourced series of expectations on them (with higher frequency, e.g. monthly)</t>
+  </si>
+  <si>
+    <t>Updated: Feb 28, 2025 7:44 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 28, 2025 11:41 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 13, 2025 7:57 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 13, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Jan 30, 2025 11:01 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Dec 19, 2024 11:01 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 20, 2025 11:01 AM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 20, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Mar 3, 2025 1:32 PM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Apr 1, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Feb 14, 2025 7:34 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 17, 2025 2:17 PM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 17, 2025 2:15 PM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 25, 2025 12:01 PM CST</t>
+  </si>
+  <si>
+    <t>Updated: Mar 3, 2025 4:01 PM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Mar 5, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Jan 8, 2025 2:04 PM CST</t>
+  </si>
+  <si>
+    <t>Next Release Date: Apr 7, 2025</t>
+  </si>
+  <si>
+    <t>Updated: Mar 7, 2025 1:18 PM CST</t>
+  </si>
+  <si>
+    <t>Updated: Mar 7, 2025 7:46 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 17, 2025 1:53 PM CST</t>
+  </si>
+  <si>
+    <t>Updated: Feb 27, 2025 7:54 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Mar 3, 2025 3:19 PM CST</t>
+  </si>
+  <si>
+    <t>??? Strange</t>
+  </si>
+  <si>
+    <t>&gt; check out DTWEXBGS, it’s quite strange</t>
+  </si>
+  <si>
+    <t>Updated: Feb 27, 2025 7:59 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Mar 3, 2025 10:16 AM CST</t>
+  </si>
+  <si>
+    <t>&gt; keep an eye on AIRRTMFMD11</t>
+  </si>
+  <si>
+    <t>Updated: Mar 7, 2025 9:14 AM CST</t>
+  </si>
+  <si>
+    <t>Updated: Mar 7, 2025 9:07 AM CST</t>
   </si>
 </sst>
 </file>
@@ -1620,13 +1923,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="14"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1660,6 +1967,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1979,10 +2290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I145"/>
+  <dimension ref="A1:K145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I122" sqref="I122"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1992,13 +2303,14 @@
     <col min="4" max="4" width="46.21875" customWidth="1"/>
     <col min="5" max="5" width="18.5546875" customWidth="1"/>
     <col min="6" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="18" width="11.88671875" customWidth="1"/>
-    <col min="19" max="19" width="51.77734375" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" customWidth="1"/>
+    <col min="10" max="10" width="31.44140625" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="19" width="11.88671875" customWidth="1"/>
+    <col min="20" max="20" width="51.77734375" customWidth="1"/>
+    <col min="21" max="21" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>419</v>
       </c>
@@ -2023,11 +2335,12 @@
       <c r="H1" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2050,11 +2363,19 @@
         <v>427</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>459</v>
+      </c>
+      <c r="J2" t="s">
+        <v>458</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2077,10 +2398,19 @@
         <v>427</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J3" t="s">
+        <v>483</v>
+      </c>
+      <c r="K3" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2103,10 +2433,19 @@
         <v>427</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>459</v>
+      </c>
+      <c r="J4" t="s">
+        <v>553</v>
+      </c>
+      <c r="K4" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2129,10 +2468,19 @@
         <v>428</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J5" t="s">
+        <v>554</v>
+      </c>
+      <c r="K5" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2155,10 +2503,19 @@
         <v>427</v>
       </c>
       <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="J6" t="s">
+        <v>463</v>
+      </c>
+      <c r="K6" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2181,10 +2538,19 @@
         <v>427</v>
       </c>
       <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J7" t="s">
+        <v>472</v>
+      </c>
+      <c r="K7" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -2207,10 +2573,19 @@
         <v>427</v>
       </c>
       <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J8" t="s">
+        <v>472</v>
+      </c>
+      <c r="K8" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -2233,10 +2608,19 @@
         <v>428</v>
       </c>
       <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J9" t="s">
+        <v>554</v>
+      </c>
+      <c r="K9" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2259,10 +2643,19 @@
         <v>428</v>
       </c>
       <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="J10" t="s">
+        <v>556</v>
+      </c>
+      <c r="K10" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2285,10 +2678,19 @@
         <v>428</v>
       </c>
       <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="J11" t="s">
+        <v>556</v>
+      </c>
+      <c r="K11" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2311,10 +2713,19 @@
         <v>428</v>
       </c>
       <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="J12" t="s">
+        <v>556</v>
+      </c>
+      <c r="K12" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -2337,10 +2748,19 @@
         <v>428</v>
       </c>
       <c r="H13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="J13" t="s">
+        <v>557</v>
+      </c>
+      <c r="K13" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -2363,10 +2783,19 @@
         <v>428</v>
       </c>
       <c r="H14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="J14" t="s">
+        <v>557</v>
+      </c>
+      <c r="K14" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2389,10 +2818,19 @@
         <v>428</v>
       </c>
       <c r="H15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="J15" t="s">
+        <v>557</v>
+      </c>
+      <c r="K15" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -2415,10 +2853,19 @@
         <v>427</v>
       </c>
       <c r="H16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="J16" t="s">
+        <v>467</v>
+      </c>
+      <c r="K16" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -2441,10 +2888,19 @@
         <v>427</v>
       </c>
       <c r="H17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J17" t="s">
+        <v>470</v>
+      </c>
+      <c r="K17" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2467,10 +2923,19 @@
         <v>427</v>
       </c>
       <c r="H18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J18" t="s">
+        <v>472</v>
+      </c>
+      <c r="K18" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2493,10 +2958,19 @@
         <v>428</v>
       </c>
       <c r="H19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J19" t="s">
+        <v>473</v>
+      </c>
+      <c r="K19" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2519,10 +2993,19 @@
         <v>428</v>
       </c>
       <c r="H20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J20" t="s">
+        <v>473</v>
+      </c>
+      <c r="K20" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -2545,10 +3028,19 @@
         <v>427</v>
       </c>
       <c r="H21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J21" t="s">
+        <v>476</v>
+      </c>
+      <c r="K21" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -2571,10 +3063,19 @@
         <v>427</v>
       </c>
       <c r="H22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="J22" t="s">
+        <v>477</v>
+      </c>
+      <c r="K22" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -2597,10 +3098,19 @@
         <v>427</v>
       </c>
       <c r="H23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J23" t="s">
+        <v>479</v>
+      </c>
+      <c r="K23" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -2623,10 +3133,19 @@
         <v>428</v>
       </c>
       <c r="H24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J24" t="s">
+        <v>480</v>
+      </c>
+      <c r="K24" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -2649,10 +3168,19 @@
         <v>428</v>
       </c>
       <c r="H25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J25" t="s">
+        <v>476</v>
+      </c>
+      <c r="K25" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -2675,10 +3203,19 @@
         <v>428</v>
       </c>
       <c r="H26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>2024</v>
+      </c>
+      <c r="J26" t="s">
+        <v>481</v>
+      </c>
+      <c r="K26" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -2701,10 +3238,19 @@
         <v>427</v>
       </c>
       <c r="H27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J27" t="s">
+        <v>483</v>
+      </c>
+      <c r="K27" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -2727,10 +3273,19 @@
         <v>427</v>
       </c>
       <c r="H28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J28" t="s">
+        <v>483</v>
+      </c>
+      <c r="K28" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -2753,10 +3308,19 @@
         <v>427</v>
       </c>
       <c r="H29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="J29" t="s">
+        <v>485</v>
+      </c>
+      <c r="K29" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -2779,10 +3343,19 @@
         <v>427</v>
       </c>
       <c r="H30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="J30" t="s">
+        <v>485</v>
+      </c>
+      <c r="K30" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -2805,10 +3378,19 @@
         <v>428</v>
       </c>
       <c r="H31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>2024</v>
+      </c>
+      <c r="J31" t="s">
+        <v>481</v>
+      </c>
+      <c r="K31" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -2831,10 +3413,19 @@
         <v>427</v>
       </c>
       <c r="H32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="J32" t="s">
+        <v>485</v>
+      </c>
+      <c r="K32" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>93</v>
       </c>
@@ -2857,10 +3448,19 @@
         <v>427</v>
       </c>
       <c r="H33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J33" t="s">
+        <v>483</v>
+      </c>
+      <c r="K33" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>96</v>
       </c>
@@ -2883,10 +3483,19 @@
         <v>428</v>
       </c>
       <c r="H34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>2024</v>
+      </c>
+      <c r="J34" t="s">
+        <v>481</v>
+      </c>
+      <c r="K34" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -2911,8 +3520,17 @@
       <c r="H35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="J35" t="s">
+        <v>487</v>
+      </c>
+      <c r="K35" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>102</v>
       </c>
@@ -2935,10 +3553,19 @@
         <v>428</v>
       </c>
       <c r="H36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="J36" t="s">
+        <v>487</v>
+      </c>
+      <c r="K36" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>105</v>
       </c>
@@ -2961,10 +3588,19 @@
         <v>427</v>
       </c>
       <c r="H37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J37" t="s">
+        <v>488</v>
+      </c>
+      <c r="K37" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -2987,10 +3623,19 @@
         <v>427</v>
       </c>
       <c r="H38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J38" t="s">
+        <v>470</v>
+      </c>
+      <c r="K38" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>111</v>
       </c>
@@ -3013,10 +3658,19 @@
         <v>428</v>
       </c>
       <c r="H39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J39" t="s">
+        <v>489</v>
+      </c>
+      <c r="K39" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>114</v>
       </c>
@@ -3039,10 +3693,19 @@
         <v>428</v>
       </c>
       <c r="H40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J40" t="s">
+        <v>490</v>
+      </c>
+      <c r="K40" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>117</v>
       </c>
@@ -3065,10 +3728,19 @@
         <v>428</v>
       </c>
       <c r="H41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J41" t="s">
+        <v>494</v>
+      </c>
+      <c r="K41" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>120</v>
       </c>
@@ -3093,8 +3765,17 @@
       <c r="H42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="J42" t="s">
+        <v>495</v>
+      </c>
+      <c r="K42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>123</v>
       </c>
@@ -3117,10 +3798,19 @@
         <v>428</v>
       </c>
       <c r="H43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J43" t="s">
+        <v>497</v>
+      </c>
+      <c r="K43" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>126</v>
       </c>
@@ -3143,10 +3833,19 @@
         <v>427</v>
       </c>
       <c r="H44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J44" t="s">
+        <v>498</v>
+      </c>
+      <c r="K44" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>129</v>
       </c>
@@ -3169,10 +3868,19 @@
         <v>428</v>
       </c>
       <c r="H45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>2023</v>
+      </c>
+      <c r="J45" t="s">
+        <v>499</v>
+      </c>
+      <c r="K45" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>132</v>
       </c>
@@ -3195,10 +3903,19 @@
         <v>428</v>
       </c>
       <c r="H46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J46" t="s">
+        <v>500</v>
+      </c>
+      <c r="K46" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>135</v>
       </c>
@@ -3221,10 +3938,19 @@
         <v>428</v>
       </c>
       <c r="H47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J47" t="s">
+        <v>500</v>
+      </c>
+      <c r="K47" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>138</v>
       </c>
@@ -3247,10 +3973,19 @@
         <v>427</v>
       </c>
       <c r="H48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="J48" t="s">
+        <v>501</v>
+      </c>
+      <c r="K48" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>141</v>
       </c>
@@ -3275,8 +4010,17 @@
       <c r="H49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="J49" t="s">
+        <v>501</v>
+      </c>
+      <c r="K49" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>144</v>
       </c>
@@ -3299,10 +4043,19 @@
         <v>428</v>
       </c>
       <c r="H50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J50" t="s">
+        <v>502</v>
+      </c>
+      <c r="K50" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>147</v>
       </c>
@@ -3327,8 +4080,17 @@
       <c r="H51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="J51" t="s">
+        <v>495</v>
+      </c>
+      <c r="K51" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>150</v>
       </c>
@@ -3353,8 +4115,17 @@
       <c r="H52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="J52" t="s">
+        <v>504</v>
+      </c>
+      <c r="K52" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>153</v>
       </c>
@@ -3377,10 +4148,19 @@
         <v>427</v>
       </c>
       <c r="H53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="J53" t="s">
+        <v>501</v>
+      </c>
+      <c r="K53" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>156</v>
       </c>
@@ -3403,10 +4183,19 @@
         <v>428</v>
       </c>
       <c r="H54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J54" t="s">
+        <v>473</v>
+      </c>
+      <c r="K54" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>159</v>
       </c>
@@ -3429,10 +4218,19 @@
         <v>428</v>
       </c>
       <c r="H55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J55" t="s">
+        <v>473</v>
+      </c>
+      <c r="K55" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>162</v>
       </c>
@@ -3455,10 +4253,19 @@
         <v>428</v>
       </c>
       <c r="H56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J56" t="s">
+        <v>473</v>
+      </c>
+      <c r="K56" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>165</v>
       </c>
@@ -3481,10 +4288,19 @@
         <v>428</v>
       </c>
       <c r="H57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J57" t="s">
+        <v>473</v>
+      </c>
+      <c r="K57" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>168</v>
       </c>
@@ -3507,10 +4323,19 @@
         <v>428</v>
       </c>
       <c r="H58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J58" t="s">
+        <v>473</v>
+      </c>
+      <c r="K58" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>171</v>
       </c>
@@ -3533,10 +4358,19 @@
         <v>428</v>
       </c>
       <c r="H59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J59" t="s">
+        <v>473</v>
+      </c>
+      <c r="K59" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>174</v>
       </c>
@@ -3559,10 +4393,19 @@
         <v>428</v>
       </c>
       <c r="H60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J60" t="s">
+        <v>473</v>
+      </c>
+      <c r="K60" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>177</v>
       </c>
@@ -3585,10 +4428,19 @@
         <v>428</v>
       </c>
       <c r="H61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="I61" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="J61" t="s">
+        <v>506</v>
+      </c>
+      <c r="K61" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>180</v>
       </c>
@@ -3611,10 +4463,19 @@
         <v>428</v>
       </c>
       <c r="H62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J62" t="s">
+        <v>509</v>
+      </c>
+      <c r="K62" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>183</v>
       </c>
@@ -3637,10 +4498,19 @@
         <v>428</v>
       </c>
       <c r="H63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I63" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="J63" t="s">
+        <v>511</v>
+      </c>
+      <c r="K63" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>186</v>
       </c>
@@ -3663,10 +4533,19 @@
         <v>428</v>
       </c>
       <c r="H64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I64" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="J64" t="s">
+        <v>511</v>
+      </c>
+      <c r="K64" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>189</v>
       </c>
@@ -3689,10 +4568,19 @@
         <v>428</v>
       </c>
       <c r="H65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I65" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="J65" t="s">
+        <v>511</v>
+      </c>
+      <c r="K65" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>192</v>
       </c>
@@ -3715,10 +4603,19 @@
         <v>428</v>
       </c>
       <c r="H66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I66" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="J66" t="s">
+        <v>511</v>
+      </c>
+      <c r="K66" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>195</v>
       </c>
@@ -3741,10 +4638,19 @@
         <v>428</v>
       </c>
       <c r="H67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J67" t="s">
+        <v>514</v>
+      </c>
+      <c r="K67" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>198</v>
       </c>
@@ -3767,10 +4673,19 @@
         <v>428</v>
       </c>
       <c r="H68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="J68" t="s">
+        <v>515</v>
+      </c>
+      <c r="K68" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>201</v>
       </c>
@@ -3793,10 +4708,19 @@
         <v>428</v>
       </c>
       <c r="H69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="J69" t="s">
+        <v>516</v>
+      </c>
+      <c r="K69" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>204</v>
       </c>
@@ -3821,8 +4745,17 @@
       <c r="H70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J70" t="s">
+        <v>518</v>
+      </c>
+      <c r="K70" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>207</v>
       </c>
@@ -3846,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>210</v>
       </c>
@@ -3869,10 +4802,19 @@
         <v>428</v>
       </c>
       <c r="H72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="J72" t="s">
+        <v>519</v>
+      </c>
+      <c r="K72" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>213</v>
       </c>
@@ -3895,10 +4837,19 @@
         <v>428</v>
       </c>
       <c r="H73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I73" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J73" t="s">
+        <v>521</v>
+      </c>
+      <c r="K73" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>216</v>
       </c>
@@ -3921,10 +4872,19 @@
         <v>427</v>
       </c>
       <c r="H74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I74" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J74" t="s">
+        <v>470</v>
+      </c>
+      <c r="K74" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>219</v>
       </c>
@@ -3947,10 +4907,19 @@
         <v>428</v>
       </c>
       <c r="H75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I75" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J75" t="s">
+        <v>522</v>
+      </c>
+      <c r="K75" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>222</v>
       </c>
@@ -3973,10 +4942,19 @@
         <v>427</v>
       </c>
       <c r="H76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I76" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="J76" t="s">
+        <v>523</v>
+      </c>
+      <c r="K76" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>225</v>
       </c>
@@ -3999,10 +4977,19 @@
         <v>428</v>
       </c>
       <c r="H77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="J77" t="s">
+        <v>523</v>
+      </c>
+      <c r="K77" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>228</v>
       </c>
@@ -4025,10 +5012,19 @@
         <v>428</v>
       </c>
       <c r="H78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I78" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="J78" t="s">
+        <v>525</v>
+      </c>
+      <c r="K78" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>231</v>
       </c>
@@ -4051,10 +5047,19 @@
         <v>427</v>
       </c>
       <c r="H79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I79" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="J79" t="s">
+        <v>470</v>
+      </c>
+      <c r="K79" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>234</v>
       </c>
@@ -4077,10 +5082,19 @@
         <v>427</v>
       </c>
       <c r="H80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I80" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J80" t="s">
+        <v>528</v>
+      </c>
+      <c r="K80" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>237</v>
       </c>
@@ -4103,10 +5117,19 @@
         <v>427</v>
       </c>
       <c r="H81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I81" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J81" t="s">
+        <v>528</v>
+      </c>
+      <c r="K81" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>240</v>
       </c>
@@ -4129,10 +5152,19 @@
         <v>427</v>
       </c>
       <c r="H82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J82" t="s">
+        <v>483</v>
+      </c>
+      <c r="K82" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>243</v>
       </c>
@@ -4155,10 +5187,19 @@
         <v>427</v>
       </c>
       <c r="H83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I83" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J83" t="s">
+        <v>483</v>
+      </c>
+      <c r="K83" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>246</v>
       </c>
@@ -4181,10 +5222,19 @@
         <v>427</v>
       </c>
       <c r="H84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I84" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J84" t="s">
+        <v>528</v>
+      </c>
+      <c r="K84" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>249</v>
       </c>
@@ -4207,10 +5257,19 @@
         <v>427</v>
       </c>
       <c r="H85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I85" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J85" t="s">
+        <v>483</v>
+      </c>
+      <c r="K85" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>252</v>
       </c>
@@ -4233,10 +5292,19 @@
         <v>427</v>
       </c>
       <c r="H86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J86" t="s">
+        <v>528</v>
+      </c>
+      <c r="K86" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>255</v>
       </c>
@@ -4259,10 +5327,19 @@
         <v>427</v>
       </c>
       <c r="H87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I87" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J87" t="s">
+        <v>529</v>
+      </c>
+      <c r="K87" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>258</v>
       </c>
@@ -4285,10 +5362,19 @@
         <v>428</v>
       </c>
       <c r="H88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J88" t="s">
+        <v>530</v>
+      </c>
+      <c r="K88" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>261</v>
       </c>
@@ -4311,10 +5397,19 @@
         <v>428</v>
       </c>
       <c r="H89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I89" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J89" t="s">
+        <v>530</v>
+      </c>
+      <c r="K89" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>264</v>
       </c>
@@ -4337,10 +5432,19 @@
         <v>428</v>
       </c>
       <c r="H90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I90" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J90" t="s">
+        <v>530</v>
+      </c>
+      <c r="K90" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>267</v>
       </c>
@@ -4363,10 +5467,19 @@
         <v>428</v>
       </c>
       <c r="H91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I91" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J91" t="s">
+        <v>530</v>
+      </c>
+      <c r="K91" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>270</v>
       </c>
@@ -4389,10 +5502,19 @@
         <v>428</v>
       </c>
       <c r="H92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I92" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J92" t="s">
+        <v>530</v>
+      </c>
+      <c r="K92" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>273</v>
       </c>
@@ -4415,10 +5537,19 @@
         <v>427</v>
       </c>
       <c r="H93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I93" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J93" t="s">
+        <v>483</v>
+      </c>
+      <c r="K93" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>276</v>
       </c>
@@ -4441,10 +5572,19 @@
         <v>427</v>
       </c>
       <c r="H94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I94" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="J94" t="s">
+        <v>501</v>
+      </c>
+      <c r="K94" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>279</v>
       </c>
@@ -4467,10 +5607,19 @@
         <v>427</v>
       </c>
       <c r="H95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I95" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="J95" t="s">
+        <v>501</v>
+      </c>
+      <c r="K95" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>282</v>
       </c>
@@ -4493,10 +5642,19 @@
         <v>427</v>
       </c>
       <c r="H96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I96" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J96" t="s">
+        <v>483</v>
+      </c>
+      <c r="K96" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>285</v>
       </c>
@@ -4519,10 +5677,19 @@
         <v>428</v>
       </c>
       <c r="H97">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I97" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="J97" t="s">
+        <v>532</v>
+      </c>
+      <c r="K97" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>288</v>
       </c>
@@ -4547,8 +5714,17 @@
       <c r="H98">
         <v>2</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="J98" t="s">
+        <v>533</v>
+      </c>
+      <c r="K98" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>291</v>
       </c>
@@ -4571,10 +5747,19 @@
         <v>427</v>
       </c>
       <c r="H99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I99" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="J99" t="s">
+        <v>463</v>
+      </c>
+      <c r="K99" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>294</v>
       </c>
@@ -4597,10 +5782,19 @@
         <v>428</v>
       </c>
       <c r="H100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I100" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="J100" t="s">
+        <v>463</v>
+      </c>
+      <c r="K100" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>297</v>
       </c>
@@ -4623,10 +5817,19 @@
         <v>428</v>
       </c>
       <c r="H101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I101" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J101" t="s">
+        <v>534</v>
+      </c>
+      <c r="K101" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>300</v>
       </c>
@@ -4649,10 +5852,19 @@
         <v>428</v>
       </c>
       <c r="H102">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I102" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J102" t="s">
+        <v>536</v>
+      </c>
+      <c r="K102" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>303</v>
       </c>
@@ -4677,8 +5889,17 @@
       <c r="H103">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J103" t="s">
+        <v>538</v>
+      </c>
+      <c r="K103" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>306</v>
       </c>
@@ -4701,10 +5922,19 @@
         <v>428</v>
       </c>
       <c r="H104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I104" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J104" t="s">
+        <v>539</v>
+      </c>
+      <c r="K104" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>309</v>
       </c>
@@ -4727,10 +5957,19 @@
         <v>428</v>
       </c>
       <c r="H105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I105" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J105" t="s">
+        <v>518</v>
+      </c>
+      <c r="K105" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>312</v>
       </c>
@@ -4753,10 +5992,19 @@
         <v>428</v>
       </c>
       <c r="H106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I106" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J106" t="s">
+        <v>518</v>
+      </c>
+      <c r="K106" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>315</v>
       </c>
@@ -4779,10 +6027,19 @@
         <v>428</v>
       </c>
       <c r="H107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I107" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J107" t="s">
+        <v>518</v>
+      </c>
+      <c r="K107" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>318</v>
       </c>
@@ -4805,10 +6062,19 @@
         <v>428</v>
       </c>
       <c r="H108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I108" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J108" t="s">
+        <v>518</v>
+      </c>
+      <c r="K108" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>321</v>
       </c>
@@ -4831,10 +6097,19 @@
         <v>428</v>
       </c>
       <c r="H109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I109" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J109" t="s">
+        <v>518</v>
+      </c>
+      <c r="K109" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>324</v>
       </c>
@@ -4857,10 +6132,19 @@
         <v>428</v>
       </c>
       <c r="H110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I110" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J110" t="s">
+        <v>518</v>
+      </c>
+      <c r="K110" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>327</v>
       </c>
@@ -4883,10 +6167,19 @@
         <v>428</v>
       </c>
       <c r="H111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I111" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J111" t="s">
+        <v>518</v>
+      </c>
+      <c r="K111" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>330</v>
       </c>
@@ -4909,10 +6202,19 @@
         <v>428</v>
       </c>
       <c r="H112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I112" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J112" t="s">
+        <v>518</v>
+      </c>
+      <c r="K112" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>333</v>
       </c>
@@ -4935,10 +6237,19 @@
         <v>428</v>
       </c>
       <c r="H113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I113" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J113" t="s">
+        <v>540</v>
+      </c>
+      <c r="K113" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>336</v>
       </c>
@@ -4961,10 +6272,19 @@
         <v>428</v>
       </c>
       <c r="H114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I114" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J114" t="s">
+        <v>540</v>
+      </c>
+      <c r="K114" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>339</v>
       </c>
@@ -4987,10 +6307,19 @@
         <v>428</v>
       </c>
       <c r="H115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I115" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J115" t="s">
+        <v>540</v>
+      </c>
+      <c r="K115" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>342</v>
       </c>
@@ -5013,10 +6342,19 @@
         <v>428</v>
       </c>
       <c r="H116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I116" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J116" t="s">
+        <v>540</v>
+      </c>
+      <c r="K116" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>345</v>
       </c>
@@ -5039,10 +6377,19 @@
         <v>427</v>
       </c>
       <c r="H117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I117" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J117" t="s">
+        <v>541</v>
+      </c>
+      <c r="K117" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>348</v>
       </c>
@@ -5065,10 +6412,19 @@
         <v>427</v>
       </c>
       <c r="H118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I118" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J118" t="s">
+        <v>498</v>
+      </c>
+      <c r="K118" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>351</v>
       </c>
@@ -5091,10 +6447,19 @@
         <v>428</v>
       </c>
       <c r="H119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I119" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J119" t="s">
+        <v>542</v>
+      </c>
+      <c r="K119" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>354</v>
       </c>
@@ -5117,10 +6482,19 @@
         <v>428</v>
       </c>
       <c r="H120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I120" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J120" t="s">
+        <v>542</v>
+      </c>
+      <c r="K120" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>357</v>
       </c>
@@ -5143,10 +6517,19 @@
         <v>428</v>
       </c>
       <c r="H121">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I121" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="J121" t="s">
+        <v>544</v>
+      </c>
+      <c r="K121" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>360</v>
       </c>
@@ -5169,10 +6552,19 @@
         <v>428</v>
       </c>
       <c r="H122">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I122" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="J122" t="s">
+        <v>544</v>
+      </c>
+      <c r="K122" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>363</v>
       </c>
@@ -5196,7 +6588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>365</v>
       </c>
@@ -5219,10 +6611,19 @@
         <v>427</v>
       </c>
       <c r="H124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I124" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J124" t="s">
+        <v>546</v>
+      </c>
+      <c r="K124" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>368</v>
       </c>
@@ -5245,10 +6646,19 @@
         <v>427</v>
       </c>
       <c r="H125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I125" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="J125" t="s">
+        <v>463</v>
+      </c>
+      <c r="K125" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>371</v>
       </c>
@@ -5271,10 +6681,19 @@
         <v>427</v>
       </c>
       <c r="H126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I126" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J126" t="s">
+        <v>547</v>
+      </c>
+      <c r="K126" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>374</v>
       </c>
@@ -5297,10 +6716,19 @@
         <v>428</v>
       </c>
       <c r="H127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I127" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="J127" t="s">
+        <v>548</v>
+      </c>
+      <c r="K127" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>377</v>
       </c>
@@ -5323,10 +6751,19 @@
         <v>428</v>
       </c>
       <c r="H128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I128" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J128" t="s">
+        <v>494</v>
+      </c>
+      <c r="K128" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>380</v>
       </c>
@@ -5349,10 +6786,19 @@
         <v>427</v>
       </c>
       <c r="H129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I129" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="J129" t="s">
+        <v>470</v>
+      </c>
+      <c r="K129" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>383</v>
       </c>
@@ -5377,8 +6823,17 @@
       <c r="H130">
         <v>2</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I130" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="J130" t="s">
+        <v>549</v>
+      </c>
+      <c r="K130" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>386</v>
       </c>
@@ -5404,7 +6859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>389</v>
       </c>
@@ -5430,7 +6885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>392</v>
       </c>
@@ -5456,7 +6911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>395</v>
       </c>
@@ -5482,7 +6937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>398</v>
       </c>
@@ -5508,7 +6963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>401</v>
       </c>
@@ -5534,7 +6989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>404</v>
       </c>
@@ -5560,7 +7015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>407</v>
       </c>
@@ -5586,7 +7041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>410</v>
       </c>
@@ -5612,7 +7067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>413</v>
       </c>
@@ -5638,7 +7093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>416</v>
       </c>
@@ -5664,7 +7119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>436</v>
       </c>
@@ -5690,7 +7145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>437</v>
       </c>
@@ -5716,7 +7171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>451</v>
       </c>
@@ -5742,7 +7197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>453</v>
       </c>
@@ -5765,11 +7220,20 @@
         <v>428</v>
       </c>
       <c r="H145">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I145" t="s">
+        <v>551</v>
+      </c>
+      <c r="J145" t="s">
+        <v>550</v>
+      </c>
+      <c r="K145" t="s">
+        <v>474</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:I340">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:J340">
     <sortCondition ref="A8:A340"/>
   </sortState>
   <hyperlinks>
@@ -5877,24 +7341,24 @@
     <hyperlink ref="D110" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
     <hyperlink ref="D111" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
     <hyperlink ref="D112" r:id="rId104" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="D113" r:id="rId105" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="D114" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="D115" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="D116" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="D117" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="D118" r:id="rId110" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="D119" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="D120" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="D121" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="D122" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="D124" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="D125" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="D126" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="D127" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="D128" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="D129" r:id="rId120" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="D130" r:id="rId121" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="D20" r:id="rId122" xr:uid="{DE32A080-980B-4A38-B062-8A8A9316BB93}"/>
+    <hyperlink ref="D114" r:id="rId105" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="D115" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="D116" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="D117" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="D118" r:id="rId109" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="D119" r:id="rId110" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="D120" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="D121" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="D122" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="D124" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="D125" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="D126" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="D127" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="D128" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="D129" r:id="rId119" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="D130" r:id="rId120" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="D20" r:id="rId121" xr:uid="{DE32A080-980B-4A38-B062-8A8A9316BB93}"/>
+    <hyperlink ref="D113" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.39370078740157505" bottom="0.39370078740157505" header="0" footer="0"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId123"/>
@@ -5907,10 +7371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DF86C7-82B7-4F6E-939E-BF588D52CF27}">
-  <dimension ref="B4:C10"/>
+  <dimension ref="B4:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5950,6 +7414,46 @@
         <v>443</v>
       </c>
     </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>555</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>